<commit_message>
Agrego los datos para las gráficas y los datos ordenando con los mismos datos
</commit_message>
<xml_diff>
--- a/TareaArchOrd/Estadisticas/Estadisticas.xlsx
+++ b/TareaArchOrd/Estadisticas/Estadisticas.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>n</t>
   </si>
@@ -28,9 +28,6 @@
   </si>
   <si>
     <t>Intercambios</t>
-  </si>
-  <si>
-    <t>te</t>
   </si>
   <si>
     <t xml:space="preserve">Tiempo de ejecución</t>
@@ -76,11 +73,10 @@
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="1" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -609,12 +605,6 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" t="s">
-        <v>0</v>
-      </c>
     </row>
     <row r="2" ht="14.25">
       <c r="A2">
@@ -629,14 +619,6 @@
       <c r="D2">
         <v>34</v>
       </c>
-      <c r="F2">
-        <f>B2*1000</f>
-        <v>0.01</v>
-      </c>
-      <c r="G2">
-        <f>A2/1000000</f>
-        <v>1.0000000000000001e-05</v>
-      </c>
     </row>
     <row r="3" ht="14.25">
       <c r="A3">
@@ -651,14 +633,7 @@
       <c r="D3">
         <v>672</v>
       </c>
-      <c r="F3" s="1">
-        <f>B3*1000</f>
-        <v>0.063</v>
-      </c>
-      <c r="G3">
-        <f>A3/1000000</f>
-        <v>0.0001</v>
-      </c>
+      <c r="F3" s="1"/>
     </row>
     <row r="4" ht="14.25">
       <c r="A4">
@@ -673,14 +648,7 @@
       <c r="D4">
         <v>9976</v>
       </c>
-      <c r="F4" s="1">
-        <f>B4*1000</f>
-        <v>0.17799999999999999</v>
-      </c>
-      <c r="G4">
-        <f>A4/1000000</f>
-        <v>0.001</v>
-      </c>
+      <c r="F4" s="1"/>
     </row>
     <row r="5" ht="14.25">
       <c r="A5">
@@ -695,14 +663,7 @@
       <c r="D5">
         <v>133616</v>
       </c>
-      <c r="F5" s="1">
-        <f>B5*1000</f>
-        <v>3.4580000000000002</v>
-      </c>
-      <c r="G5">
-        <f>A5/1000000</f>
-        <v>0.01</v>
-      </c>
+      <c r="F5" s="1"/>
     </row>
     <row r="6" ht="14.25">
       <c r="A6">
@@ -717,14 +678,7 @@
       <c r="D6">
         <v>19951424</v>
       </c>
-      <c r="F6" s="1">
-        <f>B6*1000</f>
-        <v>191.672</v>
-      </c>
-      <c r="G6">
-        <f>A6/1000000</f>
-        <v>1</v>
-      </c>
+      <c r="F6" s="1"/>
     </row>
     <row r="9" ht="14.25">
       <c r="A9" t="s">
@@ -744,13 +698,13 @@
       <c r="A10">
         <v>10</v>
       </c>
-      <c r="B10">
-        <v>1.0000000000000001e-05</v>
-      </c>
-      <c r="C10">
-        <v>21</v>
-      </c>
-      <c r="D10">
+      <c r="B10" s="1">
+        <v>6.9999999999999999e-06</v>
+      </c>
+      <c r="C10" s="1">
+        <v>22</v>
+      </c>
+      <c r="D10" s="1">
         <v>34</v>
       </c>
     </row>
@@ -758,13 +712,13 @@
       <c r="A11">
         <v>20</v>
       </c>
-      <c r="B11">
-        <v>6.9999999999999999e-06</v>
-      </c>
-      <c r="C11">
-        <v>62</v>
-      </c>
-      <c r="D11">
+      <c r="B11" s="1">
+        <v>9.0000000000000002e-06</v>
+      </c>
+      <c r="C11" s="1">
+        <v>64</v>
+      </c>
+      <c r="D11" s="1">
         <v>88</v>
       </c>
     </row>
@@ -772,13 +726,13 @@
       <c r="A12">
         <v>30</v>
       </c>
-      <c r="B12">
-        <v>1.0000000000000001e-05</v>
-      </c>
-      <c r="C12">
+      <c r="B12" s="1">
+        <v>1.1e-05</v>
+      </c>
+      <c r="C12" s="1">
         <v>108</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="1">
         <v>148</v>
       </c>
     </row>
@@ -786,13 +740,13 @@
       <c r="A13" s="2">
         <v>40</v>
       </c>
-      <c r="B13">
+      <c r="B13" s="1">
         <v>1.2999999999999999e-05</v>
       </c>
-      <c r="C13">
-        <v>167</v>
-      </c>
-      <c r="D13">
+      <c r="C13" s="1">
+        <v>165</v>
+      </c>
+      <c r="D13" s="1">
         <v>216</v>
       </c>
     </row>
@@ -800,13 +754,13 @@
       <c r="A14" s="2">
         <v>50</v>
       </c>
-      <c r="B14">
-        <v>1.2999999999999999e-05</v>
-      </c>
-      <c r="C14">
-        <v>220</v>
-      </c>
-      <c r="D14">
+      <c r="B14" s="1">
+        <v>1.5e-05</v>
+      </c>
+      <c r="C14" s="1">
+        <v>219</v>
+      </c>
+      <c r="D14" s="1">
         <v>286</v>
       </c>
     </row>
@@ -814,13 +768,13 @@
       <c r="A15" s="2">
         <v>60</v>
       </c>
-      <c r="B15">
-        <v>1.5999999999999999e-05</v>
-      </c>
-      <c r="C15">
-        <v>275</v>
-      </c>
-      <c r="D15">
+      <c r="B15" s="1">
+        <v>1.7e-05</v>
+      </c>
+      <c r="C15" s="1">
+        <v>278</v>
+      </c>
+      <c r="D15" s="1">
         <v>356</v>
       </c>
     </row>
@@ -828,13 +782,13 @@
       <c r="A16" s="2">
         <v>70</v>
       </c>
-      <c r="B16">
-        <v>2.0000000000000002e-05</v>
-      </c>
-      <c r="C16">
-        <v>340</v>
-      </c>
-      <c r="D16">
+      <c r="B16" s="1">
+        <v>2.4000000000000001e-05</v>
+      </c>
+      <c r="C16" s="1">
+        <v>344</v>
+      </c>
+      <c r="D16" s="1">
         <v>432</v>
       </c>
     </row>
@@ -842,13 +796,13 @@
       <c r="A17" s="2">
         <v>80</v>
       </c>
-      <c r="B17">
-        <v>2.4000000000000001e-05</v>
-      </c>
-      <c r="C17">
-        <v>406</v>
-      </c>
-      <c r="D17">
+      <c r="B17" s="1">
+        <v>3.3000000000000003e-05</v>
+      </c>
+      <c r="C17" s="1">
+        <v>412</v>
+      </c>
+      <c r="D17" s="1">
         <v>512</v>
       </c>
     </row>
@@ -856,13 +810,13 @@
       <c r="A18" s="2">
         <v>90</v>
       </c>
-      <c r="B18">
-        <v>2.5999999999999998e-05</v>
-      </c>
-      <c r="C18">
-        <v>465</v>
-      </c>
-      <c r="D18">
+      <c r="B18" s="1">
+        <v>3.6000000000000001e-05</v>
+      </c>
+      <c r="C18" s="1">
+        <v>471</v>
+      </c>
+      <c r="D18" s="1">
         <v>592</v>
       </c>
     </row>
@@ -870,13 +824,13 @@
       <c r="A19">
         <v>100</v>
       </c>
-      <c r="B19">
-        <v>6.3e-05</v>
-      </c>
-      <c r="C19">
-        <v>549</v>
-      </c>
-      <c r="D19">
+      <c r="B19" s="1">
+        <v>3.6000000000000001e-05</v>
+      </c>
+      <c r="C19" s="1">
+        <v>530</v>
+      </c>
+      <c r="D19" s="1">
         <v>672</v>
       </c>
     </row>
@@ -884,13 +838,13 @@
       <c r="A20">
         <v>200</v>
       </c>
-      <c r="B20">
-        <v>0.00011900000000000001</v>
-      </c>
-      <c r="C20">
-        <v>1251</v>
-      </c>
-      <c r="D20">
+      <c r="B20" s="1">
+        <v>5.3000000000000001e-05</v>
+      </c>
+      <c r="C20" s="1">
+        <v>1272</v>
+      </c>
+      <c r="D20" s="1">
         <v>1544</v>
       </c>
     </row>
@@ -898,13 +852,13 @@
       <c r="A21">
         <v>300</v>
       </c>
-      <c r="B21">
-        <v>0.000183</v>
-      </c>
-      <c r="C21">
-        <v>2065</v>
-      </c>
-      <c r="D21">
+      <c r="B21" s="1">
+        <v>8.3999999999999995e-05</v>
+      </c>
+      <c r="C21" s="1">
+        <v>2075</v>
+      </c>
+      <c r="D21" s="1">
         <v>2488</v>
       </c>
     </row>
@@ -912,13 +866,13 @@
       <c r="A22">
         <v>400</v>
       </c>
-      <c r="B22">
-        <v>0.000263</v>
-      </c>
-      <c r="C22">
-        <v>2920</v>
-      </c>
-      <c r="D22">
+      <c r="B22" s="1">
+        <v>0.00011</v>
+      </c>
+      <c r="C22" s="1">
+        <v>2892</v>
+      </c>
+      <c r="D22" s="1">
         <v>3488</v>
       </c>
     </row>
@@ -926,13 +880,13 @@
       <c r="A23">
         <v>500</v>
       </c>
-      <c r="B23">
-        <v>0.00033500000000000001</v>
-      </c>
-      <c r="C23">
-        <v>3803</v>
-      </c>
-      <c r="D23">
+      <c r="B23" s="1">
+        <v>0.00013799999999999999</v>
+      </c>
+      <c r="C23" s="1">
+        <v>3785</v>
+      </c>
+      <c r="D23" s="1">
         <v>4488</v>
       </c>
     </row>
@@ -940,13 +894,13 @@
       <c r="A24">
         <v>600</v>
       </c>
-      <c r="B24">
-        <v>0.000377</v>
-      </c>
-      <c r="C24">
-        <v>4687</v>
-      </c>
-      <c r="D24">
+      <c r="B24" s="1">
+        <v>0.000183</v>
+      </c>
+      <c r="C24" s="1">
+        <v>4698</v>
+      </c>
+      <c r="D24" s="1">
         <v>5576</v>
       </c>
     </row>
@@ -954,13 +908,13 @@
       <c r="A25">
         <v>700</v>
       </c>
-      <c r="B25">
-        <v>0.00047399999999999997</v>
-      </c>
-      <c r="C25">
-        <v>5645</v>
-      </c>
-      <c r="D25">
+      <c r="B25" s="1">
+        <v>0.000175</v>
+      </c>
+      <c r="C25" s="1">
+        <v>5611</v>
+      </c>
+      <c r="D25" s="1">
         <v>6676</v>
       </c>
     </row>
@@ -968,13 +922,13 @@
       <c r="A26">
         <v>800</v>
       </c>
-      <c r="B26">
-        <v>0.00025999999999999998</v>
-      </c>
-      <c r="C26">
-        <v>6572</v>
-      </c>
-      <c r="D26">
+      <c r="B26" s="1">
+        <v>0.00022699999999999999</v>
+      </c>
+      <c r="C26" s="1">
+        <v>6544</v>
+      </c>
+      <c r="D26" s="1">
         <v>7776</v>
       </c>
     </row>
@@ -982,13 +936,13 @@
       <c r="A27">
         <v>900</v>
       </c>
-      <c r="B27">
-        <v>0.00020799999999999999</v>
-      </c>
-      <c r="C27">
-        <v>7512</v>
-      </c>
-      <c r="D27">
+      <c r="B27" s="1">
+        <v>0.00020100000000000001</v>
+      </c>
+      <c r="C27" s="1">
+        <v>7498</v>
+      </c>
+      <c r="D27" s="1">
         <v>8876</v>
       </c>
     </row>
@@ -996,13 +950,13 @@
       <c r="A28">
         <v>1000</v>
       </c>
-      <c r="B28">
-        <v>0.00017799999999999999</v>
-      </c>
-      <c r="C28">
-        <v>8552</v>
-      </c>
-      <c r="D28">
+      <c r="B28" s="1">
+        <v>0.000224</v>
+      </c>
+      <c r="C28" s="1">
+        <v>8505</v>
+      </c>
+      <c r="D28" s="1">
         <v>9976</v>
       </c>
     </row>
@@ -1010,13 +964,13 @@
       <c r="A29">
         <v>2000</v>
       </c>
-      <c r="B29">
-        <v>0.00094600000000000001</v>
-      </c>
-      <c r="C29">
-        <v>18906</v>
-      </c>
-      <c r="D29">
+      <c r="B29" s="1">
+        <v>0.00053499999999999999</v>
+      </c>
+      <c r="C29" s="1">
+        <v>18931</v>
+      </c>
+      <c r="D29" s="1">
         <v>21952</v>
       </c>
     </row>
@@ -1024,27 +978,27 @@
       <c r="A30">
         <v>3000</v>
       </c>
-      <c r="B30">
-        <v>0.0015250000000000001</v>
-      </c>
-      <c r="C30">
-        <v>30045</v>
-      </c>
-      <c r="D30">
+      <c r="B30" s="1">
+        <v>0.00095</v>
+      </c>
+      <c r="C30" s="1">
+        <v>30120</v>
+      </c>
+      <c r="D30" s="1">
         <v>34904</v>
       </c>
     </row>
     <row r="31" ht="14.25">
-      <c r="A31" s="3">
+      <c r="A31" s="1">
         <v>4000</v>
       </c>
-      <c r="B31">
-        <v>0.001173</v>
-      </c>
-      <c r="C31">
-        <v>41754</v>
-      </c>
-      <c r="D31">
+      <c r="B31" s="1">
+        <v>0.00090899999999999998</v>
+      </c>
+      <c r="C31" s="1">
+        <v>41787</v>
+      </c>
+      <c r="D31" s="1">
         <v>47904</v>
       </c>
     </row>
@@ -1052,13 +1006,13 @@
       <c r="A32">
         <v>5000</v>
       </c>
-      <c r="B32">
-        <v>0.001348</v>
-      </c>
-      <c r="C32">
-        <v>53649</v>
-      </c>
-      <c r="D32">
+      <c r="B32" s="1">
+        <v>0.00092800000000000001</v>
+      </c>
+      <c r="C32" s="1">
+        <v>53737</v>
+      </c>
+      <c r="D32" s="1">
         <v>61808</v>
       </c>
     </row>
@@ -1066,41 +1020,41 @@
       <c r="A33">
         <v>6000</v>
       </c>
-      <c r="B33">
-        <v>0.001041</v>
-      </c>
-      <c r="C33">
-        <v>65713</v>
-      </c>
-      <c r="D33">
+      <c r="B33" s="1">
+        <v>0.0010679999999999999</v>
+      </c>
+      <c r="C33" s="1">
+        <v>65820</v>
+      </c>
+      <c r="D33" s="1">
         <v>75808</v>
       </c>
     </row>
     <row r="34" ht="14.25">
-      <c r="A34" s="3">
+      <c r="A34" s="1">
         <v>7000</v>
       </c>
-      <c r="B34">
-        <v>0.001065</v>
-      </c>
-      <c r="C34">
-        <v>78266</v>
-      </c>
-      <c r="D34">
+      <c r="B34" s="1">
+        <v>0.001256</v>
+      </c>
+      <c r="C34" s="1">
+        <v>78272</v>
+      </c>
+      <c r="D34" s="1">
         <v>89808</v>
       </c>
     </row>
     <row r="35" ht="14.25">
-      <c r="A35" s="3">
+      <c r="A35" s="1">
         <v>8000</v>
       </c>
-      <c r="B35">
-        <v>0.0014289999999999999</v>
-      </c>
-      <c r="C35">
-        <v>91038</v>
-      </c>
-      <c r="D35">
+      <c r="B35" s="1">
+        <v>0.0014369999999999999</v>
+      </c>
+      <c r="C35" s="1">
+        <v>91050</v>
+      </c>
+      <c r="D35" s="1">
         <v>103808</v>
       </c>
     </row>
@@ -1108,13 +1062,13 @@
       <c r="A36">
         <v>9000</v>
       </c>
-      <c r="B36">
-        <v>0.0014300000000000001</v>
-      </c>
-      <c r="C36">
-        <v>104076</v>
-      </c>
-      <c r="D36">
+      <c r="B36" s="1">
+        <v>0.001738</v>
+      </c>
+      <c r="C36" s="1">
+        <v>103838</v>
+      </c>
+      <c r="D36" s="1">
         <v>118616</v>
       </c>
     </row>
@@ -1122,13 +1076,13 @@
       <c r="A37">
         <v>10000</v>
       </c>
-      <c r="B37">
-        <v>0.0034580000000000001</v>
-      </c>
-      <c r="C37">
-        <v>116854</v>
-      </c>
-      <c r="D37">
+      <c r="B37" s="1">
+        <v>0.0019449999999999999</v>
+      </c>
+      <c r="C37" s="1">
+        <v>116777</v>
+      </c>
+      <c r="D37" s="1">
         <v>133616</v>
       </c>
     </row>
@@ -1136,13 +1090,13 @@
       <c r="A38">
         <v>20000</v>
       </c>
-      <c r="B38">
-        <v>0.007502</v>
-      </c>
-      <c r="C38">
-        <v>252657</v>
-      </c>
-      <c r="D38">
+      <c r="B38" s="1">
+        <v>0.00562</v>
+      </c>
+      <c r="C38" s="1">
+        <v>253106</v>
+      </c>
+      <c r="D38" s="1">
         <v>287232</v>
       </c>
     </row>
@@ -1150,13 +1104,13 @@
       <c r="A39">
         <v>30000</v>
       </c>
-      <c r="B39">
-        <v>0.0071850000000000004</v>
-      </c>
-      <c r="C39">
-        <v>395625</v>
-      </c>
-      <c r="D39">
+      <c r="B39" s="1">
+        <v>0.0063920000000000001</v>
+      </c>
+      <c r="C39" s="1">
+        <v>395919</v>
+      </c>
+      <c r="D39" s="1">
         <v>447232</v>
       </c>
     </row>
@@ -1164,27 +1118,27 @@
       <c r="A40">
         <v>40000</v>
       </c>
-      <c r="B40">
-        <v>0.0061809999999999999</v>
-      </c>
-      <c r="C40">
-        <v>543764</v>
-      </c>
-      <c r="D40">
+      <c r="B40" s="1">
+        <v>0.0067580000000000001</v>
+      </c>
+      <c r="C40" s="1">
+        <v>543463</v>
+      </c>
+      <c r="D40" s="1">
         <v>614464</v>
       </c>
     </row>
     <row r="41" ht="14.25">
-      <c r="A41" s="3">
+      <c r="A41" s="1">
         <v>50000</v>
       </c>
-      <c r="B41">
-        <v>0.0090320000000000001</v>
-      </c>
-      <c r="C41">
-        <v>694700</v>
-      </c>
-      <c r="D41">
+      <c r="B41" s="1">
+        <v>0.0079719999999999999</v>
+      </c>
+      <c r="C41" s="1">
+        <v>694614</v>
+      </c>
+      <c r="D41" s="1">
         <v>784464</v>
       </c>
     </row>
@@ -1192,13 +1146,13 @@
       <c r="A42">
         <v>60000</v>
       </c>
-      <c r="B42">
-        <v>0.010357</v>
-      </c>
-      <c r="C42">
-        <v>848795</v>
-      </c>
-      <c r="D42">
+      <c r="B42" s="1">
+        <v>0.0096159999999999995</v>
+      </c>
+      <c r="C42" s="1">
+        <v>849593</v>
+      </c>
+      <c r="D42" s="1">
         <v>954464</v>
       </c>
     </row>
@@ -1206,13 +1160,13 @@
       <c r="A43">
         <v>70000</v>
       </c>
-      <c r="B43">
-        <v>0.011885</v>
-      </c>
-      <c r="C43">
-        <v>1005843</v>
-      </c>
-      <c r="D43">
+      <c r="B43" s="1">
+        <v>0.011431</v>
+      </c>
+      <c r="C43" s="1">
+        <v>1005816</v>
+      </c>
+      <c r="D43" s="1">
         <v>1128928</v>
       </c>
     </row>
@@ -1220,27 +1174,27 @@
       <c r="A44">
         <v>80000</v>
       </c>
-      <c r="B44">
-        <v>0.013202</v>
-      </c>
-      <c r="C44">
-        <v>1163968</v>
-      </c>
-      <c r="D44">
+      <c r="B44" s="1">
+        <v>0.013991</v>
+      </c>
+      <c r="C44" s="1">
+        <v>1164079</v>
+      </c>
+      <c r="D44" s="1">
         <v>1308928</v>
       </c>
     </row>
     <row r="45" ht="14.25">
-      <c r="A45" s="3">
+      <c r="A45" s="1">
         <v>90000</v>
       </c>
-      <c r="B45">
-        <v>0.015134999999999999</v>
-      </c>
-      <c r="C45">
-        <v>1324123</v>
-      </c>
-      <c r="D45">
+      <c r="B45" s="1">
+        <v>0.014866000000000001</v>
+      </c>
+      <c r="C45" s="1">
+        <v>1324681</v>
+      </c>
+      <c r="D45" s="1">
         <v>1488928</v>
       </c>
     </row>
@@ -1248,13 +1202,13 @@
       <c r="A46">
         <v>100000</v>
       </c>
-      <c r="B46">
-        <v>0.017929</v>
-      </c>
-      <c r="C46">
-        <v>1485412</v>
-      </c>
-      <c r="D46">
+      <c r="B46" s="1">
+        <v>0.016834999999999999</v>
+      </c>
+      <c r="C46" s="1">
+        <v>1485387</v>
+      </c>
+      <c r="D46" s="1">
         <v>1668928</v>
       </c>
     </row>
@@ -1262,13 +1216,13 @@
       <c r="A47">
         <v>200000</v>
       </c>
-      <c r="B47">
-        <v>0.036804999999999997</v>
-      </c>
-      <c r="C47">
-        <v>3161459</v>
-      </c>
-      <c r="D47">
+      <c r="B47" s="1">
+        <v>0.037478999999999998</v>
+      </c>
+      <c r="C47" s="1">
+        <v>3162085</v>
+      </c>
+      <c r="D47" s="1">
         <v>3537856</v>
       </c>
     </row>
@@ -1276,13 +1230,13 @@
       <c r="A48">
         <v>300000</v>
       </c>
-      <c r="B48">
-        <v>0.054908999999999999</v>
-      </c>
-      <c r="C48">
-        <v>4909289</v>
-      </c>
-      <c r="D48">
+      <c r="B48" s="1">
+        <v>0.053830999999999997</v>
+      </c>
+      <c r="C48" s="1">
+        <v>4911429</v>
+      </c>
+      <c r="D48" s="1">
         <v>5475712</v>
       </c>
     </row>
@@ -1290,13 +1244,13 @@
       <c r="A49">
         <v>400000</v>
       </c>
-      <c r="B49">
-        <v>0.077354000000000006</v>
-      </c>
-      <c r="C49">
-        <v>6706336</v>
-      </c>
-      <c r="D49">
+      <c r="B49" s="1">
+        <v>0.075129000000000001</v>
+      </c>
+      <c r="C49" s="1">
+        <v>6704964</v>
+      </c>
+      <c r="D49" s="1">
         <v>7475712</v>
       </c>
     </row>
@@ -1304,13 +1258,13 @@
       <c r="A50">
         <v>500000</v>
       </c>
-      <c r="B50">
-        <v>0.092796000000000003</v>
-      </c>
-      <c r="C50">
-        <v>8536143</v>
-      </c>
-      <c r="D50">
+      <c r="B50" s="1">
+        <v>0.091220999999999997</v>
+      </c>
+      <c r="C50" s="1">
+        <v>8534440</v>
+      </c>
+      <c r="D50" s="1">
         <v>9475712</v>
       </c>
     </row>
@@ -1318,13 +1272,13 @@
       <c r="A51">
         <v>600000</v>
       </c>
-      <c r="B51">
-        <v>0.113769</v>
-      </c>
-      <c r="C51">
-        <v>10391990</v>
-      </c>
-      <c r="D51">
+      <c r="B51" s="1">
+        <v>0.110362</v>
+      </c>
+      <c r="C51" s="1">
+        <v>10392591</v>
+      </c>
+      <c r="D51" s="1">
         <v>11551424</v>
       </c>
     </row>
@@ -1332,13 +1286,13 @@
       <c r="A52">
         <v>700000</v>
       </c>
-      <c r="B52">
-        <v>0.13358900000000001</v>
-      </c>
-      <c r="C52">
-        <v>12275715</v>
-      </c>
-      <c r="D52">
+      <c r="B52" s="1">
+        <v>0.13323199999999999</v>
+      </c>
+      <c r="C52" s="1">
+        <v>12273778</v>
+      </c>
+      <c r="D52" s="1">
         <v>13651424</v>
       </c>
     </row>
@@ -1346,13 +1300,13 @@
       <c r="A53">
         <v>800000</v>
       </c>
-      <c r="B53">
-        <v>0.15362700000000001</v>
-      </c>
-      <c r="C53">
-        <v>14178234</v>
-      </c>
-      <c r="D53">
+      <c r="B53" s="1">
+        <v>0.15041399999999999</v>
+      </c>
+      <c r="C53" s="1">
+        <v>14172951</v>
+      </c>
+      <c r="D53" s="1">
         <v>15751424</v>
       </c>
     </row>
@@ -1360,13 +1314,13 @@
       <c r="A54">
         <v>900000</v>
       </c>
-      <c r="B54">
-        <v>0.17525499999999999</v>
-      </c>
-      <c r="C54">
-        <v>16093205</v>
-      </c>
-      <c r="D54">
+      <c r="B54" s="1">
+        <v>0.16972599999999999</v>
+      </c>
+      <c r="C54" s="1">
+        <v>16090845</v>
+      </c>
+      <c r="D54" s="1">
         <v>17851424</v>
       </c>
     </row>
@@ -1374,48 +1328,26 @@
       <c r="A55">
         <v>1000000</v>
       </c>
-      <c r="B55">
-        <v>0.19708300000000001</v>
-      </c>
-      <c r="C55">
-        <v>18027257</v>
-      </c>
-      <c r="D55">
+      <c r="B55" s="1">
+        <v>0.19265699999999999</v>
+      </c>
+      <c r="C55" s="1">
+        <v>18022771</v>
+      </c>
+      <c r="D55" s="1">
         <v>19951424</v>
       </c>
     </row>
-    <row r="56" ht="14.25">
-      <c r="B56"/>
-      <c r="C56"/>
-      <c r="D56"/>
-    </row>
+    <row r="56" ht="14.25"/>
     <row r="57" ht="14.25"/>
-    <row r="58" ht="14.25">
-      <c r="B58"/>
-      <c r="C58"/>
-      <c r="D58"/>
-    </row>
+    <row r="58" ht="14.25"/>
     <row r="59" ht="14.25"/>
-    <row r="60" ht="14.25">
-      <c r="B60"/>
-      <c r="C60"/>
-      <c r="D60"/>
-    </row>
+    <row r="60" ht="14.25"/>
     <row r="61" ht="14.25"/>
-    <row r="62" ht="14.25">
-      <c r="B62"/>
-      <c r="C62"/>
-      <c r="D62"/>
-    </row>
+    <row r="62" ht="14.25"/>
     <row r="63" ht="14.25"/>
-    <row r="64" ht="14.25">
-      <c r="B64"/>
-      <c r="C64"/>
-      <c r="D64"/>
-    </row>
-    <row r="65" ht="14.25">
-      <c r="A65"/>
-    </row>
+    <row r="64" ht="14.25"/>
+    <row r="65" ht="14.25"/>
   </sheetData>
   <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>
@@ -1431,13 +1363,17 @@
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="9.140625"/>
     <col bestFit="1" min="2" max="2" width="18.28125"/>
-    <col bestFit="1" min="3" max="3" width="14.00390625"/>
-    <col bestFit="1" min="4" max="4" width="12.00390625"/>
-    <col min="5" max="16384" width="9.140625"/>
+    <col customWidth="1" min="3" max="3" width="14.8515625"/>
+    <col customWidth="1" min="4" max="4" width="16.00390625"/>
+    <col min="5" max="6" width="9.140625"/>
+    <col bestFit="1" min="7" max="7" width="18.28125"/>
+    <col bestFit="1" customWidth="1" min="8" max="8" width="14.00390625"/>
+    <col bestFit="1" min="9" max="9" width="12.00390625"/>
+    <col min="10" max="16384" width="9.140625"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1445,12 +1381,24 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1458,83 +1406,143 @@
       <c r="A2">
         <v>10</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="1">
         <v>3.9999999999999998e-06</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="1">
         <v>34</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="1">
         <v>30</v>
+      </c>
+      <c r="F2" s="1">
+        <v>10</v>
+      </c>
+      <c r="G2" s="1">
+        <v>6.9999999999999999e-06</v>
+      </c>
+      <c r="H2" s="1">
+        <v>20</v>
+      </c>
+      <c r="I2" s="1">
+        <v>11</v>
       </c>
     </row>
     <row r="3">
       <c r="A3">
         <v>20</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="1">
         <v>5.0000000000000004e-06</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="1">
         <v>144</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="1">
         <v>127</v>
+      </c>
+      <c r="F3" s="1">
+        <v>100</v>
+      </c>
+      <c r="G3" s="1">
+        <v>4.6e-05</v>
+      </c>
+      <c r="H3" s="1">
+        <v>2251</v>
+      </c>
+      <c r="I3" s="1">
+        <v>2153</v>
       </c>
     </row>
     <row r="4">
       <c r="A4">
         <v>30</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="1">
         <v>5.0000000000000004e-06</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="1">
         <v>195</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="1">
         <v>168</v>
+      </c>
+      <c r="F4" s="1">
+        <v>1000</v>
+      </c>
+      <c r="G4" s="1">
+        <v>0.0032109999999999999</v>
+      </c>
+      <c r="H4" s="1">
+        <v>238997</v>
+      </c>
+      <c r="I4" s="1">
+        <v>237999</v>
       </c>
     </row>
     <row r="5">
       <c r="A5">
         <v>40</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="1">
         <v>6.0000000000000002e-06</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="1">
         <v>300</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="1">
         <v>261</v>
+      </c>
+      <c r="F5" s="1">
+        <v>10000</v>
+      </c>
+      <c r="G5" s="1">
+        <v>0.11139300000000001</v>
+      </c>
+      <c r="H5" s="1">
+        <v>22861585</v>
+      </c>
+      <c r="I5" s="1">
+        <v>22851589</v>
       </c>
     </row>
     <row r="6">
       <c r="A6">
         <v>50</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="1">
         <v>1.2e-05</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="1">
         <v>626</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="1">
         <v>580</v>
+      </c>
+      <c r="F6" s="1">
+        <v>1000000</v>
+      </c>
+      <c r="G6" s="1">
+        <v>1029.824883</v>
+      </c>
+      <c r="H6" s="1">
+        <v>227172707442</v>
+      </c>
+      <c r="I6" s="1">
+        <v>227171707444</v>
       </c>
     </row>
     <row r="7">
       <c r="A7">
         <v>60</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="1">
         <v>1.5999999999999999e-05</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="1">
         <v>915</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="1">
         <v>857</v>
       </c>
     </row>
@@ -1542,13 +1550,13 @@
       <c r="A8">
         <v>70</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="1">
         <v>2.4000000000000001e-05</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="1">
         <v>1237</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="1">
         <v>1172</v>
       </c>
     </row>
@@ -1556,13 +1564,13 @@
       <c r="A9">
         <v>80</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="1">
         <v>2.3e-05</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="1">
         <v>1452</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="1">
         <v>1376</v>
       </c>
     </row>
@@ -1570,13 +1578,13 @@
       <c r="A10">
         <v>90</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="1">
         <v>3.0000000000000001e-05</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="1">
         <v>1803</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="1">
         <v>1716</v>
       </c>
     </row>
@@ -1584,13 +1592,13 @@
       <c r="A11">
         <v>100</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="1">
         <v>3.8000000000000002e-05</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="1">
         <v>2394</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="1">
         <v>2296</v>
       </c>
     </row>
@@ -1598,13 +1606,13 @@
       <c r="A12">
         <v>200</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="1">
         <v>0.00011</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="1">
         <v>9279</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="1">
         <v>9083</v>
       </c>
     </row>
@@ -1612,13 +1620,13 @@
       <c r="A13">
         <v>300</v>
       </c>
-      <c r="B13">
+      <c r="B13" s="1">
         <v>0.00034000000000000002</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="1">
         <v>21120</v>
       </c>
-      <c r="D13">
+      <c r="D13" s="1">
         <v>20822</v>
       </c>
     </row>
@@ -1626,13 +1634,13 @@
       <c r="A14">
         <v>400</v>
       </c>
-      <c r="B14">
+      <c r="B14" s="1">
         <v>0.00043199999999999998</v>
       </c>
-      <c r="C14">
+      <c r="C14" s="1">
         <v>33541</v>
       </c>
-      <c r="D14">
+      <c r="D14" s="1">
         <v>33145</v>
       </c>
     </row>
@@ -1640,13 +1648,13 @@
       <c r="A15">
         <v>500</v>
       </c>
-      <c r="B15">
+      <c r="B15" s="1">
         <v>0.00071199999999999996</v>
       </c>
-      <c r="C15">
+      <c r="C15" s="1">
         <v>58363</v>
       </c>
-      <c r="D15">
+      <c r="D15" s="1">
         <v>57865</v>
       </c>
     </row>
@@ -1654,13 +1662,13 @@
       <c r="A16">
         <v>600</v>
       </c>
-      <c r="B16">
+      <c r="B16" s="1">
         <v>0.0010169999999999999</v>
       </c>
-      <c r="C16">
+      <c r="C16" s="1">
         <v>78670</v>
       </c>
-      <c r="D16">
+      <c r="D16" s="1">
         <v>78074</v>
       </c>
     </row>
@@ -1668,13 +1676,13 @@
       <c r="A17">
         <v>700</v>
       </c>
-      <c r="B17">
+      <c r="B17" s="1">
         <v>0.001096</v>
       </c>
-      <c r="C17">
+      <c r="C17" s="1">
         <v>118378</v>
       </c>
-      <c r="D17">
+      <c r="D17" s="1">
         <v>117680</v>
       </c>
     </row>
@@ -1682,13 +1690,13 @@
       <c r="A18">
         <v>800</v>
       </c>
-      <c r="B18">
+      <c r="B18" s="1">
         <v>0.00085800000000000004</v>
       </c>
-      <c r="C18">
+      <c r="C18" s="1">
         <v>148369</v>
       </c>
-      <c r="D18">
+      <c r="D18" s="1">
         <v>147573</v>
       </c>
     </row>
@@ -1696,13 +1704,13 @@
       <c r="A19">
         <v>900</v>
       </c>
-      <c r="B19">
+      <c r="B19" s="1">
         <v>0.001059</v>
       </c>
-      <c r="C19">
+      <c r="C19" s="1">
         <v>183696</v>
       </c>
-      <c r="D19">
+      <c r="D19" s="1">
         <v>182800</v>
       </c>
     </row>
@@ -1710,13 +1718,13 @@
       <c r="A20">
         <v>1000</v>
       </c>
-      <c r="B20">
+      <c r="B20" s="1">
         <v>0.001356</v>
       </c>
-      <c r="C20">
+      <c r="C20" s="1">
         <v>236104</v>
       </c>
-      <c r="D20">
+      <c r="D20" s="1">
         <v>235106</v>
       </c>
     </row>
@@ -1724,13 +1732,13 @@
       <c r="A21">
         <v>2000</v>
       </c>
-      <c r="B21">
+      <c r="B21" s="1">
         <v>0.005561</v>
       </c>
-      <c r="C21">
+      <c r="C21" s="1">
         <v>918396</v>
       </c>
-      <c r="D21">
+      <c r="D21" s="1">
         <v>916398</v>
       </c>
     </row>
@@ -1738,13 +1746,13 @@
       <c r="A22">
         <v>3000</v>
       </c>
-      <c r="B22">
+      <c r="B22" s="1">
         <v>0.010533000000000001</v>
       </c>
-      <c r="C22">
+      <c r="C22" s="1">
         <v>2017101</v>
       </c>
-      <c r="D22">
+      <c r="D22" s="1">
         <v>2014107</v>
       </c>
     </row>
@@ -1752,13 +1760,13 @@
       <c r="A23">
         <v>4000</v>
       </c>
-      <c r="B23">
+      <c r="B23" s="1">
         <v>0.018173999999999999</v>
       </c>
-      <c r="C23">
+      <c r="C23" s="1">
         <v>3630164</v>
       </c>
-      <c r="D23">
+      <c r="D23" s="1">
         <v>3626165</v>
       </c>
     </row>
@@ -1766,13 +1774,13 @@
       <c r="A24">
         <v>5000</v>
       </c>
-      <c r="B24">
+      <c r="B24" s="1">
         <v>0.029019</v>
       </c>
-      <c r="C24">
+      <c r="C24" s="1">
         <v>5761198</v>
       </c>
-      <c r="D24">
+      <c r="D24" s="1">
         <v>5756201</v>
       </c>
     </row>
@@ -1780,13 +1788,13 @@
       <c r="A25">
         <v>6000</v>
       </c>
-      <c r="B25">
+      <c r="B25" s="1">
         <v>0.038943999999999999</v>
       </c>
-      <c r="C25">
+      <c r="C25" s="1">
         <v>8102690</v>
       </c>
-      <c r="D25">
+      <c r="D25" s="1">
         <v>8096691</v>
       </c>
     </row>
@@ -1794,13 +1802,13 @@
       <c r="A26">
         <v>7000</v>
       </c>
-      <c r="B26">
+      <c r="B26" s="1">
         <v>0.054273000000000002</v>
       </c>
-      <c r="C26">
+      <c r="C26" s="1">
         <v>11243326</v>
       </c>
-      <c r="D26">
+      <c r="D26" s="1">
         <v>11236330</v>
       </c>
     </row>
@@ -1808,13 +1816,13 @@
       <c r="A27">
         <v>8000</v>
       </c>
-      <c r="B27">
+      <c r="B27" s="1">
         <v>0.070630999999999999</v>
       </c>
-      <c r="C27">
+      <c r="C27" s="1">
         <v>14431069</v>
       </c>
-      <c r="D27">
+      <c r="D27" s="1">
         <v>14423074</v>
       </c>
     </row>
@@ -1822,13 +1830,13 @@
       <c r="A28">
         <v>9000</v>
       </c>
-      <c r="B28">
+      <c r="B28" s="1">
         <v>0.091797000000000004</v>
       </c>
-      <c r="C28">
+      <c r="C28" s="1">
         <v>18648141</v>
       </c>
-      <c r="D28">
+      <c r="D28" s="1">
         <v>18639143</v>
       </c>
     </row>
@@ -1836,13 +1844,13 @@
       <c r="A29">
         <v>10000</v>
       </c>
-      <c r="B29">
+      <c r="B29" s="1">
         <v>0.10999</v>
       </c>
-      <c r="C29">
+      <c r="C29" s="1">
         <v>22915960</v>
       </c>
-      <c r="D29">
+      <c r="D29" s="1">
         <v>22905963</v>
       </c>
     </row>
@@ -1850,13 +1858,13 @@
       <c r="A30">
         <v>20000</v>
       </c>
-      <c r="B30">
+      <c r="B30" s="1">
         <v>0.43616899999999997</v>
       </c>
-      <c r="C30">
+      <c r="C30" s="1">
         <v>91151243</v>
       </c>
-      <c r="D30">
+      <c r="D30" s="1">
         <v>91131247</v>
       </c>
     </row>
@@ -1864,13 +1872,13 @@
       <c r="A31">
         <v>30000</v>
       </c>
-      <c r="B31">
+      <c r="B31" s="1">
         <v>0.97079700000000002</v>
       </c>
-      <c r="C31">
+      <c r="C31" s="1">
         <v>204799667</v>
       </c>
-      <c r="D31">
+      <c r="D31" s="1">
         <v>204769670</v>
       </c>
     </row>
@@ -1878,13 +1886,13 @@
       <c r="A32">
         <v>40000</v>
       </c>
-      <c r="B32">
+      <c r="B32" s="1">
         <v>1.7136690000000001</v>
       </c>
-      <c r="C32">
+      <c r="C32" s="1">
         <v>363745204</v>
       </c>
-      <c r="D32">
+      <c r="D32" s="1">
         <v>363705207</v>
       </c>
     </row>
@@ -1892,13 +1900,13 @@
       <c r="A33">
         <v>50000</v>
       </c>
-      <c r="B33">
+      <c r="B33" s="1">
         <v>2.6766580000000002</v>
       </c>
-      <c r="C33">
+      <c r="C33" s="1">
         <v>565220889</v>
       </c>
-      <c r="D33">
+      <c r="D33" s="1">
         <v>565170892</v>
       </c>
     </row>
@@ -1906,13 +1914,13 @@
       <c r="A34">
         <v>60000</v>
       </c>
-      <c r="B34">
+      <c r="B34" s="1">
         <v>3.8528959999999999</v>
       </c>
-      <c r="C34">
+      <c r="C34" s="1">
         <v>814423179</v>
       </c>
-      <c r="D34">
+      <c r="D34" s="1">
         <v>814363181</v>
       </c>
     </row>
@@ -1920,13 +1928,13 @@
       <c r="A35">
         <v>70000</v>
       </c>
-      <c r="B35">
+      <c r="B35" s="1">
         <v>5.2695829999999999</v>
       </c>
-      <c r="C35">
+      <c r="C35" s="1">
         <v>1114215758</v>
       </c>
-      <c r="D35">
+      <c r="D35" s="1">
         <v>1114145762</v>
       </c>
     </row>
@@ -1934,13 +1942,13 @@
       <c r="A36">
         <v>80000</v>
       </c>
-      <c r="B36">
+      <c r="B36" s="1">
         <v>6.9016060000000001</v>
       </c>
-      <c r="C36">
+      <c r="C36" s="1">
         <v>1452507572</v>
       </c>
-      <c r="D36">
+      <c r="D36" s="1">
         <v>1452427575</v>
       </c>
     </row>
@@ -1948,13 +1956,13 @@
       <c r="A37">
         <v>90000</v>
       </c>
-      <c r="B37">
+      <c r="B37" s="1">
         <v>8.7603290000000005</v>
       </c>
-      <c r="C37">
+      <c r="C37" s="1">
         <v>1847846348</v>
       </c>
-      <c r="D37">
+      <c r="D37" s="1">
         <v>1847756349</v>
       </c>
     </row>
@@ -1962,14 +1970,140 @@
       <c r="A38">
         <v>100000</v>
       </c>
-      <c r="B38">
+      <c r="B38" s="1">
         <v>10.874197000000001</v>
       </c>
-      <c r="C38">
+      <c r="C38" s="1">
         <v>2276581322</v>
       </c>
-      <c r="D38">
+      <c r="D38" s="1">
         <v>2276481324</v>
+      </c>
+    </row>
+    <row r="39" ht="14.25">
+      <c r="A39">
+        <v>200000</v>
+      </c>
+      <c r="B39" s="1">
+        <v>40.791004000000001</v>
+      </c>
+      <c r="C39" s="1">
+        <v>9111917335</v>
+      </c>
+      <c r="D39" s="1">
+        <v>9111717339</v>
+      </c>
+    </row>
+    <row r="40" ht="14.25">
+      <c r="A40">
+        <v>300000</v>
+      </c>
+      <c r="B40" s="1">
+        <v>89.620766000000003</v>
+      </c>
+      <c r="C40" s="1">
+        <v>20443362147</v>
+      </c>
+      <c r="D40" s="1">
+        <v>20443062152</v>
+      </c>
+    </row>
+    <row r="41" ht="14.25">
+      <c r="A41">
+        <v>400000</v>
+      </c>
+      <c r="B41" s="1">
+        <v>159.17611299999999</v>
+      </c>
+      <c r="C41" s="1">
+        <v>36369654601</v>
+      </c>
+      <c r="D41" s="1">
+        <v>36369254606</v>
+      </c>
+    </row>
+    <row r="42" ht="14.25">
+      <c r="A42">
+        <v>500000</v>
+      </c>
+      <c r="B42" s="1">
+        <v>273.37684100000001</v>
+      </c>
+      <c r="C42" s="1">
+        <v>56832628732</v>
+      </c>
+      <c r="D42" s="1">
+        <v>56832128735</v>
+      </c>
+    </row>
+    <row r="43" ht="14.25">
+      <c r="A43">
+        <v>600000</v>
+      </c>
+      <c r="B43" s="1">
+        <v>400.35668399999997</v>
+      </c>
+      <c r="C43" s="1">
+        <v>81694579064</v>
+      </c>
+      <c r="D43" s="1">
+        <v>81693979068</v>
+      </c>
+    </row>
+    <row r="44" ht="14.25">
+      <c r="A44">
+        <v>700000</v>
+      </c>
+      <c r="B44" s="1">
+        <v>530.77403700000002</v>
+      </c>
+      <c r="C44" s="1">
+        <v>111466997612</v>
+      </c>
+      <c r="D44" s="1">
+        <v>111466297614</v>
+      </c>
+    </row>
+    <row r="45" ht="14.25">
+      <c r="A45">
+        <v>800000</v>
+      </c>
+      <c r="B45" s="1">
+        <v>776.34096499999998</v>
+      </c>
+      <c r="C45" s="1">
+        <v>145423832004</v>
+      </c>
+      <c r="D45" s="1">
+        <v>145423032007</v>
+      </c>
+    </row>
+    <row r="46" ht="14.25">
+      <c r="A46">
+        <v>900000</v>
+      </c>
+      <c r="B46" s="1">
+        <v>1085.4146149999999</v>
+      </c>
+      <c r="C46" s="1">
+        <v>184040110587</v>
+      </c>
+      <c r="D46" s="1">
+        <v>184039210590</v>
+      </c>
+    </row>
+    <row r="47" ht="14.25">
+      <c r="A47">
+        <v>1000000</v>
+      </c>
+      <c r="B47" s="1">
+        <v>1288.620576</v>
+      </c>
+      <c r="C47" s="1">
+        <v>227197533745</v>
+      </c>
+      <c r="D47" s="1">
+        <v>227196533749</v>
       </c>
     </row>
   </sheetData>
@@ -1987,18 +2121,22 @@
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="9.140625"/>
     <col bestFit="1" min="2" max="2" width="18.28125"/>
     <col bestFit="1" min="3" max="3" width="14.00390625"/>
     <col bestFit="1" min="4" max="4" width="12.00390625"/>
-    <col min="5" max="16384" width="9.140625"/>
+    <col min="5" max="6" width="9.140625"/>
+    <col bestFit="1" min="7" max="7" width="18.28125"/>
+    <col bestFit="1" min="8" max="8" width="14.00390625"/>
+    <col bestFit="1" min="9" max="9" width="12.00390625"/>
+    <col min="10" max="16384" width="9.140625"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
@@ -2007,6 +2145,18 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
@@ -2014,13 +2164,25 @@
       <c r="A2">
         <v>10</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="1">
         <v>3.9999999999999998e-06</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="1">
         <v>45</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="1">
+        <v>5</v>
+      </c>
+      <c r="F2" s="1">
+        <v>10</v>
+      </c>
+      <c r="G2" s="1">
+        <v>6.9999999999999999e-06</v>
+      </c>
+      <c r="H2" s="1">
+        <v>45</v>
+      </c>
+      <c r="I2" s="1">
         <v>5</v>
       </c>
     </row>
@@ -2028,69 +2190,117 @@
       <c r="A3">
         <v>20</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="1">
         <v>6.9999999999999999e-06</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="1">
         <v>190</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="1">
         <v>17</v>
+      </c>
+      <c r="F3" s="1">
+        <v>100</v>
+      </c>
+      <c r="G3" s="1">
+        <v>6.8999999999999997e-05</v>
+      </c>
+      <c r="H3" s="1">
+        <v>4950</v>
+      </c>
+      <c r="I3" s="1">
+        <v>93</v>
       </c>
     </row>
     <row r="4">
       <c r="A4">
         <v>30</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="1">
         <v>1.1e-05</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="1">
         <v>435</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="1">
         <v>25</v>
+      </c>
+      <c r="F4" s="1">
+        <v>1000</v>
+      </c>
+      <c r="G4" s="1">
+        <v>0.0014419999999999999</v>
+      </c>
+      <c r="H4" s="1">
+        <v>499500</v>
+      </c>
+      <c r="I4" s="1">
+        <v>917</v>
       </c>
     </row>
     <row r="5">
       <c r="A5">
         <v>40</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="1">
         <v>1.5e-05</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="1">
         <v>780</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="1">
         <v>35</v>
+      </c>
+      <c r="F5" s="1">
+        <v>10000</v>
+      </c>
+      <c r="G5" s="1">
+        <v>0.13647100000000001</v>
+      </c>
+      <c r="H5" s="1">
+        <v>49995000</v>
+      </c>
+      <c r="I5" s="1">
+        <v>9103</v>
       </c>
     </row>
     <row r="6">
       <c r="A6">
         <v>50</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="1">
         <v>2.0000000000000002e-05</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="1">
         <v>1225</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="1">
         <v>42</v>
+      </c>
+      <c r="F6" s="1">
+        <v>1000000</v>
+      </c>
+      <c r="G6" s="1">
+        <v>1315.765116</v>
+      </c>
+      <c r="H6" s="1">
+        <v>499999500000</v>
+      </c>
+      <c r="I6" s="1">
+        <v>909558</v>
       </c>
     </row>
     <row r="7">
       <c r="A7">
         <v>60</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="1">
         <v>3.1000000000000001e-05</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="1">
         <v>1770</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="1">
         <v>58</v>
       </c>
     </row>
@@ -2098,13 +2308,13 @@
       <c r="A8">
         <v>70</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="1">
         <v>3.6999999999999998e-05</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="1">
         <v>2415</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="1">
         <v>57</v>
       </c>
     </row>
@@ -2112,13 +2322,13 @@
       <c r="A9">
         <v>80</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="1">
         <v>4.3000000000000002e-05</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="1">
         <v>3160</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="1">
         <v>71</v>
       </c>
     </row>
@@ -2126,13 +2336,13 @@
       <c r="A10">
         <v>90</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="1">
         <v>4.3000000000000002e-05</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="1">
         <v>4005</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="1">
         <v>82</v>
       </c>
     </row>
@@ -2140,13 +2350,13 @@
       <c r="A11">
         <v>100</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="1">
         <v>5.3000000000000001e-05</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="1">
         <v>4950</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="1">
         <v>85</v>
       </c>
     </row>
@@ -2154,13 +2364,13 @@
       <c r="A12">
         <v>200</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="1">
         <v>0.00013999999999999999</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="1">
         <v>19900</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="1">
         <v>178</v>
       </c>
     </row>
@@ -2168,13 +2378,13 @@
       <c r="A13">
         <v>300</v>
       </c>
-      <c r="B13">
+      <c r="B13" s="1">
         <v>0.000415</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="1">
         <v>44850</v>
       </c>
-      <c r="D13">
+      <c r="D13" s="1">
         <v>277</v>
       </c>
     </row>
@@ -2182,13 +2392,13 @@
       <c r="A14">
         <v>400</v>
       </c>
-      <c r="B14">
+      <c r="B14" s="1">
         <v>0.000629</v>
       </c>
-      <c r="C14">
+      <c r="C14" s="1">
         <v>79800</v>
       </c>
-      <c r="D14">
+      <c r="D14" s="1">
         <v>361</v>
       </c>
     </row>
@@ -2196,13 +2406,13 @@
       <c r="A15">
         <v>500</v>
       </c>
-      <c r="B15">
+      <c r="B15" s="1">
         <v>0.00088900000000000003</v>
       </c>
-      <c r="C15">
+      <c r="C15" s="1">
         <v>124750</v>
       </c>
-      <c r="D15">
+      <c r="D15" s="1">
         <v>464</v>
       </c>
     </row>
@@ -2210,13 +2420,13 @@
       <c r="A16">
         <v>600</v>
       </c>
-      <c r="B16">
+      <c r="B16" s="1">
         <v>0.0012210000000000001</v>
       </c>
-      <c r="C16">
+      <c r="C16" s="1">
         <v>179700</v>
       </c>
-      <c r="D16">
+      <c r="D16" s="1">
         <v>548</v>
       </c>
     </row>
@@ -2224,13 +2434,13 @@
       <c r="A17">
         <v>700</v>
       </c>
-      <c r="B17">
+      <c r="B17" s="1">
         <v>0.001606</v>
       </c>
-      <c r="C17">
+      <c r="C17" s="1">
         <v>244650</v>
       </c>
-      <c r="D17">
+      <c r="D17" s="1">
         <v>621</v>
       </c>
     </row>
@@ -2238,13 +2448,13 @@
       <c r="A18">
         <v>800</v>
       </c>
-      <c r="B18">
+      <c r="B18" s="1">
         <v>0.0021189999999999998</v>
       </c>
-      <c r="C18">
+      <c r="C18" s="1">
         <v>319600</v>
       </c>
-      <c r="D18">
+      <c r="D18" s="1">
         <v>727</v>
       </c>
     </row>
@@ -2252,13 +2462,13 @@
       <c r="A19">
         <v>900</v>
       </c>
-      <c r="B19">
+      <c r="B19" s="1">
         <v>0.0021080000000000001</v>
       </c>
-      <c r="C19">
+      <c r="C19" s="1">
         <v>404550</v>
       </c>
-      <c r="D19">
+      <c r="D19" s="1">
         <v>819</v>
       </c>
     </row>
@@ -2266,13 +2476,13 @@
       <c r="A20">
         <v>1000</v>
       </c>
-      <c r="B20">
+      <c r="B20" s="1">
         <v>0.0023089999999999999</v>
       </c>
-      <c r="C20">
+      <c r="C20" s="1">
         <v>499500</v>
       </c>
-      <c r="D20">
+      <c r="D20" s="1">
         <v>900</v>
       </c>
     </row>
@@ -2280,13 +2490,13 @@
       <c r="A21">
         <v>2000</v>
       </c>
-      <c r="B21">
+      <c r="B21" s="1">
         <v>0.0076499999999999997</v>
       </c>
-      <c r="C21">
+      <c r="C21" s="1">
         <v>1999000</v>
       </c>
-      <c r="D21">
+      <c r="D21" s="1">
         <v>1817</v>
       </c>
     </row>
@@ -2294,13 +2504,13 @@
       <c r="A22">
         <v>3000</v>
       </c>
-      <c r="B22">
+      <c r="B22" s="1">
         <v>0.014674</v>
       </c>
-      <c r="C22">
+      <c r="C22" s="1">
         <v>4498500</v>
       </c>
-      <c r="D22">
+      <c r="D22" s="1">
         <v>2723</v>
       </c>
     </row>
@@ -2308,13 +2518,13 @@
       <c r="A23">
         <v>4000</v>
       </c>
-      <c r="B23">
+      <c r="B23" s="1">
         <v>0.022696000000000001</v>
       </c>
-      <c r="C23">
+      <c r="C23" s="1">
         <v>7998000</v>
       </c>
-      <c r="D23">
+      <c r="D23" s="1">
         <v>3620</v>
       </c>
     </row>
@@ -2322,13 +2532,13 @@
       <c r="A24">
         <v>5000</v>
       </c>
-      <c r="B24">
+      <c r="B24" s="1">
         <v>0.035201999999999997</v>
       </c>
-      <c r="C24">
+      <c r="C24" s="1">
         <v>12497500</v>
       </c>
-      <c r="D24">
+      <c r="D24" s="1">
         <v>4565</v>
       </c>
     </row>
@@ -2336,13 +2546,13 @@
       <c r="A25">
         <v>6000</v>
       </c>
-      <c r="B25">
+      <c r="B25" s="1">
         <v>0.051672000000000003</v>
       </c>
-      <c r="C25">
+      <c r="C25" s="1">
         <v>17997000</v>
       </c>
-      <c r="D25">
+      <c r="D25" s="1">
         <v>5453</v>
       </c>
     </row>
@@ -2350,13 +2560,13 @@
       <c r="A26">
         <v>7000</v>
       </c>
-      <c r="B26">
+      <c r="B26" s="1">
         <v>0.066961000000000007</v>
       </c>
-      <c r="C26">
+      <c r="C26" s="1">
         <v>24496500</v>
       </c>
-      <c r="D26">
+      <c r="D26" s="1">
         <v>6340</v>
       </c>
     </row>
@@ -2364,13 +2574,13 @@
       <c r="A27">
         <v>8000</v>
       </c>
-      <c r="B27">
+      <c r="B27" s="1">
         <v>0.087773000000000004</v>
       </c>
-      <c r="C27">
+      <c r="C27" s="1">
         <v>31996000</v>
       </c>
-      <c r="D27">
+      <c r="D27" s="1">
         <v>7299</v>
       </c>
     </row>
@@ -2378,13 +2588,13 @@
       <c r="A28">
         <v>9000</v>
       </c>
-      <c r="B28">
+      <c r="B28" s="1">
         <v>0.11130900000000001</v>
       </c>
-      <c r="C28">
+      <c r="C28" s="1">
         <v>40495500</v>
       </c>
-      <c r="D28">
+      <c r="D28" s="1">
         <v>8187</v>
       </c>
     </row>
@@ -2392,13 +2602,13 @@
       <c r="A29">
         <v>10000</v>
       </c>
-      <c r="B29">
+      <c r="B29" s="1">
         <v>0.137632</v>
       </c>
-      <c r="C29">
+      <c r="C29" s="1">
         <v>49995000</v>
       </c>
-      <c r="D29">
+      <c r="D29" s="1">
         <v>9098</v>
       </c>
     </row>
@@ -2406,13 +2616,13 @@
       <c r="A30">
         <v>20000</v>
       </c>
-      <c r="B30">
+      <c r="B30" s="1">
         <v>0.550261</v>
       </c>
-      <c r="C30">
+      <c r="C30" s="1">
         <v>199990000</v>
       </c>
-      <c r="D30">
+      <c r="D30" s="1">
         <v>18160</v>
       </c>
     </row>
@@ -2420,13 +2630,13 @@
       <c r="A31">
         <v>30000</v>
       </c>
-      <c r="B31">
+      <c r="B31" s="1">
         <v>1.2206459999999999</v>
       </c>
-      <c r="C31">
+      <c r="C31" s="1">
         <v>449985000</v>
       </c>
-      <c r="D31">
+      <c r="D31" s="1">
         <v>27303</v>
       </c>
     </row>
@@ -2434,13 +2644,13 @@
       <c r="A32">
         <v>40000</v>
       </c>
-      <c r="B32">
+      <c r="B32" s="1">
         <v>2.163176</v>
       </c>
-      <c r="C32">
+      <c r="C32" s="1">
         <v>799980000</v>
       </c>
-      <c r="D32">
+      <c r="D32" s="1">
         <v>36506</v>
       </c>
     </row>
@@ -2448,13 +2658,13 @@
       <c r="A33">
         <v>50000</v>
       </c>
-      <c r="B33">
+      <c r="B33" s="1">
         <v>3.3812169999999999</v>
       </c>
-      <c r="C33">
+      <c r="C33" s="1">
         <v>1249975000</v>
       </c>
-      <c r="D33">
+      <c r="D33" s="1">
         <v>45458</v>
       </c>
     </row>
@@ -2462,13 +2672,13 @@
       <c r="A34">
         <v>60000</v>
       </c>
-      <c r="B34">
+      <c r="B34" s="1">
         <v>4.8445580000000001</v>
       </c>
-      <c r="C34">
+      <c r="C34" s="1">
         <v>1799970000</v>
       </c>
-      <c r="D34">
+      <c r="D34" s="1">
         <v>54552</v>
       </c>
     </row>
@@ -2476,13 +2686,13 @@
       <c r="A35">
         <v>70000</v>
       </c>
-      <c r="B35">
+      <c r="B35" s="1">
         <v>6.5955209999999997</v>
       </c>
-      <c r="C35">
+      <c r="C35" s="1">
         <v>2449965000</v>
       </c>
-      <c r="D35">
+      <c r="D35" s="1">
         <v>63589</v>
       </c>
     </row>
@@ -2490,13 +2700,13 @@
       <c r="A36">
         <v>80000</v>
       </c>
-      <c r="B36">
+      <c r="B36" s="1">
         <v>8.6389420000000001</v>
       </c>
-      <c r="C36">
+      <c r="C36" s="1">
         <v>3199960000</v>
       </c>
-      <c r="D36">
+      <c r="D36" s="1">
         <v>72783</v>
       </c>
     </row>
@@ -2504,13 +2714,13 @@
       <c r="A37">
         <v>90000</v>
       </c>
-      <c r="B37">
+      <c r="B37" s="1">
         <v>11.140234</v>
       </c>
-      <c r="C37">
+      <c r="C37" s="1">
         <v>4049955000</v>
       </c>
-      <c r="D37">
+      <c r="D37" s="1">
         <v>81860</v>
       </c>
     </row>
@@ -2518,14 +2728,140 @@
       <c r="A38">
         <v>100000</v>
       </c>
-      <c r="B38">
+      <c r="B38" s="1">
         <v>13.747885999999999</v>
       </c>
-      <c r="C38">
+      <c r="C38" s="1">
         <v>4999950000</v>
       </c>
-      <c r="D38">
+      <c r="D38" s="1">
         <v>90762</v>
+      </c>
+    </row>
+    <row r="39" ht="14.25">
+      <c r="A39">
+        <v>200000</v>
+      </c>
+      <c r="B39" s="1">
+        <v>52.515434999999997</v>
+      </c>
+      <c r="C39" s="1">
+        <v>19999900000</v>
+      </c>
+      <c r="D39" s="1">
+        <v>181828</v>
+      </c>
+    </row>
+    <row r="40" ht="14.25">
+      <c r="A40">
+        <v>300000</v>
+      </c>
+      <c r="B40" s="1">
+        <v>118.224777</v>
+      </c>
+      <c r="C40" s="1">
+        <v>44999850000</v>
+      </c>
+      <c r="D40" s="1">
+        <v>272765</v>
+      </c>
+    </row>
+    <row r="41" ht="14.25">
+      <c r="A41">
+        <v>400000</v>
+      </c>
+      <c r="B41" s="1">
+        <v>215.88634999999999</v>
+      </c>
+      <c r="C41" s="1">
+        <v>79999800000</v>
+      </c>
+      <c r="D41" s="1">
+        <v>363743</v>
+      </c>
+    </row>
+    <row r="42" ht="14.25">
+      <c r="A42">
+        <v>500000</v>
+      </c>
+      <c r="B42" s="1">
+        <v>333.72287599999999</v>
+      </c>
+      <c r="C42" s="1">
+        <v>124999750000</v>
+      </c>
+      <c r="D42" s="1">
+        <v>454466</v>
+      </c>
+    </row>
+    <row r="43" ht="14.25">
+      <c r="A43">
+        <v>600000</v>
+      </c>
+      <c r="B43" s="1">
+        <v>476.39401600000002</v>
+      </c>
+      <c r="C43" s="1">
+        <v>179999700000</v>
+      </c>
+      <c r="D43" s="1">
+        <v>545556</v>
+      </c>
+    </row>
+    <row r="44" ht="14.25">
+      <c r="A44">
+        <v>700000</v>
+      </c>
+      <c r="B44" s="1">
+        <v>649.90525200000002</v>
+      </c>
+      <c r="C44" s="1">
+        <v>244999650000</v>
+      </c>
+      <c r="D44" s="1">
+        <v>635928</v>
+      </c>
+    </row>
+    <row r="45" ht="14.25">
+      <c r="A45">
+        <v>800000</v>
+      </c>
+      <c r="B45" s="1">
+        <v>850.55070000000001</v>
+      </c>
+      <c r="C45" s="1">
+        <v>319999600000</v>
+      </c>
+      <c r="D45" s="1">
+        <v>727528</v>
+      </c>
+    </row>
+    <row r="46" ht="14.25">
+      <c r="A46">
+        <v>900000</v>
+      </c>
+      <c r="B46" s="1">
+        <v>1076.099291</v>
+      </c>
+      <c r="C46" s="1">
+        <v>404999550000</v>
+      </c>
+      <c r="D46" s="1">
+        <v>817502</v>
+      </c>
+    </row>
+    <row r="47" ht="14.25">
+      <c r="A47">
+        <v>1000000</v>
+      </c>
+      <c r="B47" s="1">
+        <v>1317.904845</v>
+      </c>
+      <c r="C47" s="1">
+        <v>499999500000</v>
+      </c>
+      <c r="D47" s="1">
+        <v>908702</v>
       </c>
     </row>
   </sheetData>
@@ -2543,18 +2879,22 @@
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="9.140625"/>
     <col bestFit="1" min="2" max="2" width="18.28125"/>
     <col bestFit="1" min="3" max="3" width="14.00390625"/>
     <col bestFit="1" min="4" max="4" width="12.00390625"/>
-    <col min="5" max="16384" width="9.140625"/>
+    <col min="5" max="6" width="9.140625"/>
+    <col bestFit="1" min="7" max="7" width="18.28125"/>
+    <col bestFit="1" min="8" max="8" width="14.00390625"/>
+    <col bestFit="1" min="9" max="9" width="12.00390625"/>
+    <col min="10" max="16384" width="9.140625"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
@@ -2563,6 +2903,18 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
@@ -2570,83 +2922,143 @@
       <c r="A2">
         <v>10</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="1">
         <v>3.9999999999999998e-06</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="1">
         <v>45</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="1">
         <v>4</v>
+      </c>
+      <c r="F2" s="1">
+        <v>10</v>
+      </c>
+      <c r="G2" s="1">
+        <v>6.9999999999999999e-06</v>
+      </c>
+      <c r="H2" s="1">
+        <v>45</v>
+      </c>
+      <c r="I2" s="1">
+        <v>5</v>
       </c>
     </row>
     <row r="3">
       <c r="A3">
         <v>20</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="1">
         <v>7.9999999999999996e-06</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="1">
         <v>190</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="1">
         <v>17</v>
+      </c>
+      <c r="F3" s="1">
+        <v>100</v>
+      </c>
+      <c r="G3" s="1">
+        <v>5.1999999999999997e-05</v>
+      </c>
+      <c r="H3" s="1">
+        <v>4950</v>
+      </c>
+      <c r="I3" s="1">
+        <v>93</v>
       </c>
     </row>
     <row r="4">
       <c r="A4">
         <v>30</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="1">
         <v>1.1e-05</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="1">
         <v>435</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="1">
         <v>23</v>
+      </c>
+      <c r="F4" s="1">
+        <v>1000</v>
+      </c>
+      <c r="G4" s="1">
+        <v>0.0045950000000000001</v>
+      </c>
+      <c r="H4" s="1">
+        <v>499500</v>
+      </c>
+      <c r="I4" s="1">
+        <v>917</v>
       </c>
     </row>
     <row r="5">
       <c r="A5">
         <v>40</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="1">
         <v>1.5e-05</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="1">
         <v>780</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="1">
         <v>31</v>
+      </c>
+      <c r="F5" s="1">
+        <v>10000</v>
+      </c>
+      <c r="G5" s="1">
+        <v>0.14474500000000001</v>
+      </c>
+      <c r="H5" s="1">
+        <v>49995000</v>
+      </c>
+      <c r="I5" s="1">
+        <v>9103</v>
       </c>
     </row>
     <row r="6">
       <c r="A6">
         <v>50</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="1">
         <v>1.9000000000000001e-05</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="1">
         <v>1225</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="1">
         <v>42</v>
+      </c>
+      <c r="F6" s="1">
+        <v>1000000</v>
+      </c>
+      <c r="G6" s="1">
+        <v>1392.862578</v>
+      </c>
+      <c r="H6" s="1">
+        <v>499999500000</v>
+      </c>
+      <c r="I6" s="1">
+        <v>909558</v>
       </c>
     </row>
     <row r="7">
       <c r="A7">
         <v>60</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="1">
         <v>2.3e-05</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="1">
         <v>1770</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="1">
         <v>50</v>
       </c>
     </row>
@@ -2654,13 +3066,13 @@
       <c r="A8">
         <v>70</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="1">
         <v>2.8e-05</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="1">
         <v>2415</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="1">
         <v>61</v>
       </c>
     </row>
@@ -2668,13 +3080,13 @@
       <c r="A9">
         <v>80</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="1">
         <v>3.8000000000000002e-05</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="1">
         <v>3160</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="1">
         <v>73</v>
       </c>
     </row>
@@ -2682,13 +3094,13 @@
       <c r="A10">
         <v>90</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="1">
         <v>4.8999999999999998e-05</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="1">
         <v>4005</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="1">
         <v>74</v>
       </c>
     </row>
@@ -2696,13 +3108,13 @@
       <c r="A11">
         <v>100</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="1">
         <v>5.7000000000000003e-05</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="1">
         <v>4950</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="1">
         <v>89</v>
       </c>
     </row>
@@ -2710,13 +3122,13 @@
       <c r="A12">
         <v>200</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="1">
         <v>0.00017799999999999999</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="1">
         <v>19900</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="1">
         <v>182</v>
       </c>
     </row>
@@ -2724,13 +3136,13 @@
       <c r="A13">
         <v>300</v>
       </c>
-      <c r="B13">
+      <c r="B13" s="1">
         <v>0.00040499999999999998</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="1">
         <v>44850</v>
       </c>
-      <c r="D13">
+      <c r="D13" s="1">
         <v>274</v>
       </c>
     </row>
@@ -2738,13 +3150,13 @@
       <c r="A14">
         <v>400</v>
       </c>
-      <c r="B14">
+      <c r="B14" s="1">
         <v>0.00083699999999999996</v>
       </c>
-      <c r="C14">
+      <c r="C14" s="1">
         <v>79800</v>
       </c>
-      <c r="D14">
+      <c r="D14" s="1">
         <v>367</v>
       </c>
     </row>
@@ -2752,13 +3164,13 @@
       <c r="A15">
         <v>500</v>
       </c>
-      <c r="B15">
+      <c r="B15" s="1">
         <v>0.001206</v>
       </c>
-      <c r="C15">
+      <c r="C15" s="1">
         <v>124750</v>
       </c>
-      <c r="D15">
+      <c r="D15" s="1">
         <v>467</v>
       </c>
     </row>
@@ -2766,13 +3178,13 @@
       <c r="A16">
         <v>600</v>
       </c>
-      <c r="B16">
+      <c r="B16" s="1">
         <v>0.001614</v>
       </c>
-      <c r="C16">
+      <c r="C16" s="1">
         <v>179700</v>
       </c>
-      <c r="D16">
+      <c r="D16" s="1">
         <v>551</v>
       </c>
     </row>
@@ -2780,13 +3192,13 @@
       <c r="A17">
         <v>700</v>
       </c>
-      <c r="B17">
+      <c r="B17" s="1">
         <v>0.0016789999999999999</v>
       </c>
-      <c r="C17">
+      <c r="C17" s="1">
         <v>244650</v>
       </c>
-      <c r="D17">
+      <c r="D17" s="1">
         <v>635</v>
       </c>
     </row>
@@ -2794,13 +3206,13 @@
       <c r="A18">
         <v>800</v>
       </c>
-      <c r="B18">
+      <c r="B18" s="1">
         <v>0.0015590000000000001</v>
       </c>
-      <c r="C18">
+      <c r="C18" s="1">
         <v>319600</v>
       </c>
-      <c r="D18">
+      <c r="D18" s="1">
         <v>704</v>
       </c>
     </row>
@@ -2808,13 +3220,13 @@
       <c r="A19">
         <v>900</v>
       </c>
-      <c r="B19">
+      <c r="B19" s="1">
         <v>0.0018569999999999999</v>
       </c>
-      <c r="C19">
+      <c r="C19" s="1">
         <v>404550</v>
       </c>
-      <c r="D19">
+      <c r="D19" s="1">
         <v>809</v>
       </c>
     </row>
@@ -2822,13 +3234,13 @@
       <c r="A20">
         <v>1000</v>
       </c>
-      <c r="B20">
+      <c r="B20" s="1">
         <v>0.0019550000000000001</v>
       </c>
-      <c r="C20">
+      <c r="C20" s="1">
         <v>499500</v>
       </c>
-      <c r="D20">
+      <c r="D20" s="1">
         <v>905</v>
       </c>
     </row>
@@ -2836,13 +3248,13 @@
       <c r="A21">
         <v>2000</v>
       </c>
-      <c r="B21">
+      <c r="B21" s="1">
         <v>0.010881</v>
       </c>
-      <c r="C21">
+      <c r="C21" s="1">
         <v>1999000</v>
       </c>
-      <c r="D21">
+      <c r="D21" s="1">
         <v>1806</v>
       </c>
     </row>
@@ -2850,13 +3262,13 @@
       <c r="A22">
         <v>3000</v>
       </c>
-      <c r="B22">
+      <c r="B22" s="1">
         <v>0.012566000000000001</v>
       </c>
-      <c r="C22">
+      <c r="C22" s="1">
         <v>4498500</v>
       </c>
-      <c r="D22">
+      <c r="D22" s="1">
         <v>2710</v>
       </c>
     </row>
@@ -2864,13 +3276,13 @@
       <c r="A23">
         <v>4000</v>
       </c>
-      <c r="B23">
+      <c r="B23" s="1">
         <v>0.022565999999999999</v>
       </c>
-      <c r="C23">
+      <c r="C23" s="1">
         <v>7998000</v>
       </c>
-      <c r="D23">
+      <c r="D23" s="1">
         <v>3646</v>
       </c>
     </row>
@@ -2878,13 +3290,13 @@
       <c r="A24">
         <v>5000</v>
       </c>
-      <c r="B24">
+      <c r="B24" s="1">
         <v>0.034200000000000001</v>
       </c>
-      <c r="C24">
+      <c r="C24" s="1">
         <v>12497500</v>
       </c>
-      <c r="D24">
+      <c r="D24" s="1">
         <v>4542</v>
       </c>
     </row>
@@ -2892,13 +3304,13 @@
       <c r="A25">
         <v>6000</v>
       </c>
-      <c r="B25">
+      <c r="B25" s="1">
         <v>0.050221000000000002</v>
       </c>
-      <c r="C25">
+      <c r="C25" s="1">
         <v>17997000</v>
       </c>
-      <c r="D25">
+      <c r="D25" s="1">
         <v>5471</v>
       </c>
     </row>
@@ -2906,13 +3318,13 @@
       <c r="A26">
         <v>7000</v>
       </c>
-      <c r="B26">
+      <c r="B26" s="1">
         <v>0.068333000000000005</v>
       </c>
-      <c r="C26">
+      <c r="C26" s="1">
         <v>24496500</v>
       </c>
-      <c r="D26">
+      <c r="D26" s="1">
         <v>6394</v>
       </c>
     </row>
@@ -2920,13 +3332,13 @@
       <c r="A27">
         <v>8000</v>
       </c>
-      <c r="B27">
+      <c r="B27" s="1">
         <v>0.088926000000000005</v>
       </c>
-      <c r="C27">
+      <c r="C27" s="1">
         <v>31996000</v>
       </c>
-      <c r="D27">
+      <c r="D27" s="1">
         <v>7261</v>
       </c>
     </row>
@@ -2934,13 +3346,13 @@
       <c r="A28">
         <v>9000</v>
       </c>
-      <c r="B28">
+      <c r="B28" s="1">
         <v>0.11182599999999999</v>
       </c>
-      <c r="C28">
+      <c r="C28" s="1">
         <v>40495500</v>
       </c>
-      <c r="D28">
+      <c r="D28" s="1">
         <v>8166</v>
       </c>
     </row>
@@ -2948,13 +3360,13 @@
       <c r="A29">
         <v>10000</v>
       </c>
-      <c r="B29">
+      <c r="B29" s="1">
         <v>0.13697899999999999</v>
       </c>
-      <c r="C29">
+      <c r="C29" s="1">
         <v>49995000</v>
       </c>
-      <c r="D29">
+      <c r="D29" s="1">
         <v>9103</v>
       </c>
     </row>
@@ -2962,13 +3374,13 @@
       <c r="A30">
         <v>20000</v>
       </c>
-      <c r="B30">
+      <c r="B30" s="1">
         <v>0.54478499999999996</v>
       </c>
-      <c r="C30">
+      <c r="C30" s="1">
         <v>199990000</v>
       </c>
-      <c r="D30">
+      <c r="D30" s="1">
         <v>18082</v>
       </c>
     </row>
@@ -2976,13 +3388,13 @@
       <c r="A31">
         <v>30000</v>
       </c>
-      <c r="B31">
+      <c r="B31" s="1">
         <v>1.2160299999999999</v>
       </c>
-      <c r="C31">
+      <c r="C31" s="1">
         <v>449985000</v>
       </c>
-      <c r="D31">
+      <c r="D31" s="1">
         <v>27409</v>
       </c>
     </row>
@@ -2990,13 +3402,13 @@
       <c r="A32">
         <v>40000</v>
       </c>
-      <c r="B32">
+      <c r="B32" s="1">
         <v>2.1692499999999999</v>
       </c>
-      <c r="C32">
+      <c r="C32" s="1">
         <v>799980000</v>
       </c>
-      <c r="D32">
+      <c r="D32" s="1">
         <v>36316</v>
       </c>
     </row>
@@ -3004,13 +3416,13 @@
       <c r="A33">
         <v>50000</v>
       </c>
-      <c r="B33">
+      <c r="B33" s="1">
         <v>3.3729580000000001</v>
       </c>
-      <c r="C33">
+      <c r="C33" s="1">
         <v>1249975000</v>
       </c>
-      <c r="D33">
+      <c r="D33" s="1">
         <v>45420</v>
       </c>
     </row>
@@ -3018,13 +3430,13 @@
       <c r="A34">
         <v>60000</v>
       </c>
-      <c r="B34">
+      <c r="B34" s="1">
         <v>4.8518080000000001</v>
       </c>
-      <c r="C34">
+      <c r="C34" s="1">
         <v>1799970000</v>
       </c>
-      <c r="D34">
+      <c r="D34" s="1">
         <v>54513</v>
       </c>
     </row>
@@ -3032,13 +3444,13 @@
       <c r="A35">
         <v>70000</v>
       </c>
-      <c r="B35">
+      <c r="B35" s="1">
         <v>6.6035510000000004</v>
       </c>
-      <c r="C35">
+      <c r="C35" s="1">
         <v>2449965000</v>
       </c>
-      <c r="D35">
+      <c r="D35" s="1">
         <v>63518</v>
       </c>
     </row>
@@ -3046,13 +3458,13 @@
       <c r="A36">
         <v>80000</v>
       </c>
-      <c r="B36">
+      <c r="B36" s="1">
         <v>8.6215729999999997</v>
       </c>
-      <c r="C36">
+      <c r="C36" s="1">
         <v>3199960000</v>
       </c>
-      <c r="D36">
+      <c r="D36" s="1">
         <v>72682</v>
       </c>
     </row>
@@ -3060,13 +3472,13 @@
       <c r="A37">
         <v>90000</v>
       </c>
-      <c r="B37">
+      <c r="B37" s="1">
         <v>10.969234999999999</v>
       </c>
-      <c r="C37">
+      <c r="C37" s="1">
         <v>4049955000</v>
       </c>
-      <c r="D37">
+      <c r="D37" s="1">
         <v>81778</v>
       </c>
     </row>
@@ -3074,14 +3486,140 @@
       <c r="A38">
         <v>100000</v>
       </c>
-      <c r="B38">
+      <c r="B38" s="1">
         <v>13.553879</v>
       </c>
-      <c r="C38">
+      <c r="C38" s="1">
         <v>4999950000</v>
       </c>
-      <c r="D38">
+      <c r="D38" s="1">
         <v>90849</v>
+      </c>
+    </row>
+    <row r="39" ht="14.25">
+      <c r="A39">
+        <v>200000</v>
+      </c>
+      <c r="B39" s="1">
+        <v>55.195698</v>
+      </c>
+      <c r="C39" s="1">
+        <v>19999900000</v>
+      </c>
+      <c r="D39" s="1">
+        <v>181869</v>
+      </c>
+    </row>
+    <row r="40" ht="14.25">
+      <c r="A40">
+        <v>300000</v>
+      </c>
+      <c r="B40" s="1">
+        <v>124.399165</v>
+      </c>
+      <c r="C40" s="1">
+        <v>44999850000</v>
+      </c>
+      <c r="D40" s="1">
+        <v>272820</v>
+      </c>
+    </row>
+    <row r="41" ht="14.25">
+      <c r="A41">
+        <v>400000</v>
+      </c>
+      <c r="B41" s="1">
+        <v>220.87684100000001</v>
+      </c>
+      <c r="C41" s="1">
+        <v>79999800000</v>
+      </c>
+      <c r="D41" s="1">
+        <v>363239</v>
+      </c>
+    </row>
+    <row r="42" ht="14.25">
+      <c r="A42">
+        <v>500000</v>
+      </c>
+      <c r="B42" s="1">
+        <v>345.3347</v>
+      </c>
+      <c r="C42" s="1">
+        <v>124999750000</v>
+      </c>
+      <c r="D42" s="1">
+        <v>455066</v>
+      </c>
+    </row>
+    <row r="43" ht="14.25">
+      <c r="A43">
+        <v>600000</v>
+      </c>
+      <c r="B43" s="1">
+        <v>497.41929199999998</v>
+      </c>
+      <c r="C43" s="1">
+        <v>179999700000</v>
+      </c>
+      <c r="D43" s="1">
+        <v>545661</v>
+      </c>
+    </row>
+    <row r="44" ht="14.25">
+      <c r="A44">
+        <v>700000</v>
+      </c>
+      <c r="B44" s="1">
+        <v>677.51503100000002</v>
+      </c>
+      <c r="C44" s="1">
+        <v>244999650000</v>
+      </c>
+      <c r="D44" s="1">
+        <v>636418</v>
+      </c>
+    </row>
+    <row r="45" ht="14.25">
+      <c r="A45">
+        <v>800000</v>
+      </c>
+      <c r="B45" s="1">
+        <v>884.56111199999998</v>
+      </c>
+      <c r="C45" s="1">
+        <v>319999600000</v>
+      </c>
+      <c r="D45" s="1">
+        <v>727243</v>
+      </c>
+    </row>
+    <row r="46" ht="14.25">
+      <c r="A46">
+        <v>900000</v>
+      </c>
+      <c r="B46" s="1">
+        <v>1118.8950030000001</v>
+      </c>
+      <c r="C46" s="1">
+        <v>404999550000</v>
+      </c>
+      <c r="D46" s="1">
+        <v>818081</v>
+      </c>
+    </row>
+    <row r="47" ht="14.25">
+      <c r="A47">
+        <v>1000000</v>
+      </c>
+      <c r="B47" s="1">
+        <v>1382.5599910000001</v>
+      </c>
+      <c r="C47" s="1">
+        <v>499999500000</v>
+      </c>
+      <c r="D47" s="1">
+        <v>909222</v>
       </c>
     </row>
   </sheetData>

</xml_diff>